<commit_message>
new data + changed file names to reflect strain #
</commit_message>
<xml_diff>
--- a/myData/LEB 7-19-18 Strain 34 35 36.xlsx
+++ b/myData/LEB 7-19-18 Strain 34 35 36.xlsx
@@ -548,8 +548,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -623,7 +625,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -634,6 +636,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -644,6 +647,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3143,7 +3147,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:N1048576"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4834,7 +4838,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6265,6 +6269,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>